<commit_message>
Updates to Pruebas-Voraz branch
</commit_message>
<xml_diff>
--- a/pruebas Voraces.xlsx
+++ b/pruebas Voraces.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correounivalleeduco-my.sharepoint.com/personal/kevin_alejandro_velez_correounivalle_edu_co/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correounivalleeduco-my.sharepoint.com/personal/kevin_alejandro_velez_correounivalle_edu_co/Documents/Documentos/Proyectos Github/Proyecto-ADAII/Proyecto_ADA_II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="373" documentId="8_{5894B133-BE41-4873-8E6F-550ECB9AC0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B58C7C9-316D-4CCB-B81F-5222B6654002}"/>
+  <xr:revisionPtr revIDLastSave="408" documentId="8_{5894B133-BE41-4873-8E6F-550ECB9AC0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6E6F478-5430-4610-AC47-EA5811BCB031}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{560D9B95-22B0-4B72-B9AA-FB740B8357E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="91">
   <si>
     <t>Análisis Algoritmos Voraz</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t>0.134</t>
+  </si>
+  <si>
+    <t>Algoritmo 5</t>
+  </si>
+  <si>
+    <t>0.156</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>0.183</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>Juan - Alexander</t>
   </si>
 </sst>
 </file>
@@ -368,11 +386,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,13 +403,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE22F1D8-8899-4812-8E3D-09BE6A12C096}">
   <dimension ref="A2:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,10 +757,11 @@
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -761,60 +777,66 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -832,26 +854,30 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>26</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>33</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>19</v>
       </c>
       <c r="F8" s="1">
         <v>20</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -863,7 +889,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -881,26 +907,30 @@
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>27</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>35</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>37</v>
       </c>
       <c r="F11" s="1">
         <v>40</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -912,7 +942,7 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -930,26 +960,30 @@
       <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1">
         <v>118</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>124</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>96</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <v>46</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -961,7 +995,7 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -979,26 +1013,30 @@
       <c r="F16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1">
         <v>117</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="1">
         <v>117</v>
       </c>
       <c r="E17" s="1">
         <v>117</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <v>43</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1">
+        <v>117</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -1010,7 +1048,7 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1028,26 +1066,30 @@
       <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>96</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="1">
         <v>101</v>
       </c>
       <c r="E20" s="1">
         <v>113</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>41</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>113</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -1059,7 +1101,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1080,20 +1122,20 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1">
         <v>188</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="1">
         <v>189</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>187</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>126</v>
       </c>
       <c r="G23" s="1"/>
@@ -1108,7 +1150,7 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1129,20 +1171,20 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>131</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="1">
         <v>133</v>
       </c>
       <c r="E26" s="1">
         <v>138</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="6">
         <v>63</v>
       </c>
       <c r="G26" s="1"/>
@@ -1157,7 +1199,7 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1178,20 +1220,20 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="1">
         <v>345</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="1">
         <v>345</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>303</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>73</v>
       </c>
       <c r="G29" s="1"/>
@@ -1206,7 +1248,7 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1227,20 +1269,20 @@
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="1">
         <v>288</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="1">
         <v>298</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>246</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="6">
         <v>94</v>
       </c>
       <c r="G32" s="1"/>
@@ -1255,7 +1297,7 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1276,20 +1318,20 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="1">
         <v>199</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="1">
         <v>224</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="6">
         <v>231</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <v>141</v>
       </c>
       <c r="G35" s="1"/>
@@ -1304,7 +1346,7 @@
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1325,20 +1367,20 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="1">
         <v>502</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="1">
         <v>497</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>468</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="6">
         <v>70</v>
       </c>
       <c r="G38" s="1"/>
@@ -1353,7 +1395,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1374,20 +1416,20 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="1">
         <v>508</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>475</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="1">
         <v>504</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="6">
         <v>63</v>
       </c>
       <c r="G41" s="1"/>
@@ -1402,7 +1444,7 @@
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1423,20 +1465,20 @@
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="1">
         <v>392</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="1">
         <v>401</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>384</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="6">
         <v>78</v>
       </c>
       <c r="G44" s="1"/>
@@ -1451,7 +1493,7 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1472,20 +1514,20 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="8"/>
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>641</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="3">
         <v>641</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="1">
         <v>689</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="6">
         <v>77</v>
       </c>
       <c r="G47" s="1"/>
@@ -1500,7 +1542,7 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1518,26 +1560,30 @@
       <c r="F49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
+      <c r="A50" s="8"/>
       <c r="B50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="1">
         <v>1690</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="3">
         <v>1521</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="1">
         <v>1678</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="6">
         <v>175</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50" s="1">
+        <v>1868</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
@@ -1549,7 +1595,7 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1570,20 +1616,20 @@
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
+      <c r="A53" s="8"/>
       <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="1">
         <v>862</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="1">
         <v>877</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="1">
         <v>803</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="6">
         <v>81</v>
       </c>
       <c r="G53" s="1"/>
@@ -1598,7 +1644,7 @@
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1619,20 +1665,20 @@
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="3">
         <v>530</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="1">
         <v>537</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="3">
         <v>531</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="6">
         <v>81</v>
       </c>
       <c r="G56" s="1"/>
@@ -1647,7 +1693,7 @@
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1668,20 +1714,20 @@
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="1">
         <v>2383</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="1">
         <v>2383</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="3">
         <v>2120</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F59" s="6">
         <v>139</v>
       </c>
       <c r="G59" s="1"/>
@@ -1696,7 +1742,7 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1717,20 +1763,20 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="1">
         <v>1183</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="3">
         <v>1101</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="3">
         <v>1154</v>
       </c>
-      <c r="F62" s="8">
+      <c r="F62" s="6">
         <v>109</v>
       </c>
       <c r="G62" s="1"/>
@@ -1745,7 +1791,7 @@
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1766,20 +1812,20 @@
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
+      <c r="A65" s="8"/>
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="3">
         <v>1058</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="1">
         <v>1127</v>
       </c>
-      <c r="E65" s="7">
+      <c r="E65" s="1">
         <v>1158</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="6">
         <v>126</v>
       </c>
       <c r="G65" s="1"/>
@@ -1794,7 +1840,7 @@
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1815,20 +1861,20 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="3">
         <v>1184</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D68" s="3">
         <v>1227</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="3">
         <v>1227</v>
       </c>
-      <c r="F68" s="8">
+      <c r="F68" s="6">
         <v>140</v>
       </c>
       <c r="G68" s="1"/>
@@ -1843,7 +1889,7 @@
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1864,20 +1910,20 @@
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="1">
         <v>3718</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D71" s="3">
         <v>3594</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71" s="1">
         <v>3659</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="6">
         <v>261</v>
       </c>
       <c r="G71" s="1"/>
@@ -1892,7 +1938,7 @@
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1913,20 +1959,20 @@
       <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="2"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="1">
         <v>1258</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="1">
         <v>1281</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="3">
         <v>1188</v>
       </c>
-      <c r="F74" s="8">
+      <c r="F74" s="6">
         <v>96</v>
       </c>
       <c r="G74" s="1"/>
@@ -1941,7 +1987,7 @@
       <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1962,20 +2008,20 @@
       <c r="G76" s="1"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
+      <c r="A77" s="8"/>
       <c r="B77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="3">
         <v>1502</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="1">
         <v>1567</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="3">
         <v>1552</v>
       </c>
-      <c r="F77" s="8">
+      <c r="F77" s="6">
         <v>138</v>
       </c>
       <c r="G77" s="1"/>
@@ -1990,7 +2036,7 @@
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2011,20 +2057,20 @@
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="3">
         <v>2256</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="1">
         <v>2195</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="3">
         <v>2215</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F80" s="6">
         <v>188</v>
       </c>
       <c r="G80" s="1"/>
@@ -2039,7 +2085,7 @@
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2060,20 +2106,20 @@
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
+      <c r="A83" s="8"/>
       <c r="B83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="1">
         <v>4232</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D83" s="1">
         <v>3957</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="3">
         <v>3868</v>
       </c>
-      <c r="F83" s="8">
+      <c r="F83" s="6">
         <v>198</v>
       </c>
       <c r="G83" s="1"/>
@@ -2088,7 +2134,7 @@
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2109,20 +2155,20 @@
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
+      <c r="A86" s="8"/>
       <c r="B86" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="3">
         <v>3953</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D86" s="1">
         <v>3816</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="3">
         <v>3940</v>
       </c>
-      <c r="F86" s="8">
+      <c r="F86" s="6">
         <v>204</v>
       </c>
       <c r="G86" s="1"/>
@@ -2137,7 +2183,7 @@
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2158,20 +2204,20 @@
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="2"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="1">
         <v>4974</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="1">
         <v>4758</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E89" s="1">
         <v>3940</v>
       </c>
-      <c r="F89" s="8">
+      <c r="F89" s="6">
         <v>245</v>
       </c>
       <c r="G89" s="1"/>
@@ -2186,7 +2232,7 @@
       <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -2207,25 +2253,25 @@
       <c r="G91" s="1"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="2"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="1">
         <v>4982</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D92" s="1">
         <v>4993</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="3">
         <v>4965</v>
       </c>
-      <c r="F92" s="8">
+      <c r="F92" s="6">
         <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="8" t="s">
         <v>82</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2245,30 +2291,43 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="8"/>
       <c r="B95" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="3">
         <v>7520</v>
       </c>
-      <c r="D95" s="7">
+      <c r="D95" s="1">
         <v>7372</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="1">
         <v>7355</v>
       </c>
-      <c r="F95" s="8">
+      <c r="F95" s="6">
         <v>277</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A55:A56"/>
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="A64:A65"/>
@@ -2276,24 +2335,11 @@
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A91:A92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>